<commit_message>
producer with search done
</commit_message>
<xml_diff>
--- a/FlightScannerDispatcher/Data/Input/FlightTracker.xlsx
+++ b/FlightScannerDispatcher/Data/Input/FlightTracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flightSearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flightSearch\FlightScannerRpaProject\FlightScannerDispatcher\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC746D9-A6A0-40EA-A27A-94AA0A96C263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30E25C0-1BA1-4DD3-8FAB-3E6EB00B7A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A671C9B1-7234-434C-9FEE-5583EF8FDA19}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Origin</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>Day Departure</t>
+  </si>
+  <si>
+    <t>Day Arrival</t>
   </si>
 </sst>
 </file>
@@ -437,21 +449,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92848BA1-3C44-4789-A504-D83AA9324178}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,32 +476,110 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
         <v>120</v>
       </c>
     </row>

</xml_diff>